<commit_message>
Analyse des logs chgInfnegsRemet - Version 2 Evolution de CompteursFichierColl.to_excel()
</commit_message>
<xml_diff>
--- a/Excel/sample.xlsx
+++ b/Excel/sample.xlsx
@@ -6,7 +6,8 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Feuille 2" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -71,7 +72,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="2">
@@ -398,7 +399,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="2" t="n">
-        <v>42683.59377901621</v>
+        <v>43006.45625978009</v>
       </c>
       <c r="B2" t="n">
         <v>2</v>
@@ -416,4 +417,22 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>